<commit_message>
updating EXCEL file content
</commit_message>
<xml_diff>
--- a/sprints/B65 - Outil de planification et de suivi de projet.xlsx
+++ b/sprints/B65 - Outil de planification et de suivi de projet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Second\Desktop\_School-S6\B65-Synth\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Second\Desktop\_School-S6\UNOJS\sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE6CC30-F763-4B26-B9A6-F252B9039C1A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1B8B7C-F029-4466-B1D0-FFCCF217760E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="494" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="494" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Planification" sheetId="1" r:id="rId1"/>
@@ -114,18 +114,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="77">
-  <si>
-    <t>Nom du projet super cool que vous faites!</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="107">
   <si>
     <t>B65 - Projet Synthèse  |  Sprint 1  |  Planification</t>
   </si>
   <si>
     <t>Réalisé par</t>
-  </si>
-  <si>
-    <t>votre nom</t>
   </si>
   <si>
     <t>Planification</t>
@@ -396,6 +390,102 @@
   </si>
   <si>
     <t>Doute pour la creation du serveur</t>
+  </si>
+  <si>
+    <t>Daniel Pascual</t>
+  </si>
+  <si>
+    <t>UnoJS</t>
+  </si>
+  <si>
+    <t>Creer une classe deck</t>
+  </si>
+  <si>
+    <t>creer une classe hand</t>
+  </si>
+  <si>
+    <t>creer une classe joueur</t>
+  </si>
+  <si>
+    <t>creer une classe table</t>
+  </si>
+  <si>
+    <t>creer une variable globale jeu</t>
+  </si>
+  <si>
+    <t>creer une classe règles</t>
+  </si>
+  <si>
+    <t>creer un lobby</t>
+  </si>
+  <si>
+    <t>créer un menu</t>
+  </si>
+  <si>
+    <t>créer mécanique UNO</t>
+  </si>
+  <si>
+    <t>implémenter un random des cartes</t>
+  </si>
+  <si>
+    <t>créer un algorithme d'affichage des joueurs</t>
+  </si>
+  <si>
+    <t>Créer le code reliant client-serveur</t>
+  </si>
+  <si>
+    <t>Se procurer un serveur</t>
+  </si>
+  <si>
+    <t>Créer un UI de gameplay</t>
+  </si>
+  <si>
+    <t>Créer un UI pour la carte</t>
+  </si>
+  <si>
+    <t>Créer l'animation des cartes</t>
+  </si>
+  <si>
+    <t>Créer un UI pour le wild card</t>
+  </si>
+  <si>
+    <t>créer un système de point</t>
+  </si>
+  <si>
+    <t>Creer une classe mère carte</t>
+  </si>
+  <si>
+    <t>Il manque le reverse et le skip turn</t>
+  </si>
+  <si>
+    <t>Switch de html canvas à html normal puis terminer avec svelte</t>
+  </si>
+  <si>
+    <t>Fonctionne avec 2 joeurs seulement pour l'instant</t>
+  </si>
+  <si>
+    <t>Difficulté a limiter un room a 4 et quitter le socket</t>
+  </si>
+  <si>
+    <t>Comprendre socket fut plus difficile que prevu</t>
+  </si>
+  <si>
+    <t>Créer un menu d'options</t>
+  </si>
+  <si>
+    <t>J'ai fini par utiliser des boutons/select/textInput personnalisé</t>
+  </si>
+  <si>
+    <t>Petit bugs avec l'affichage</t>
+  </si>
+  <si>
+    <t>Les règles ont été déplacé dans le code du joueur et de la table</t>
+  </si>
+  <si>
+    <t>Pas assez de temps pour implémenter un menu qui change la logique de jeu</t>
+  </si>
+  <si>
+    <t>Le système de point n'est pas autant important que le UNO</t>
   </si>
 </sst>
 </file>
@@ -2664,10 +2754,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2741,10 +2831,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3087,10 +3177,10 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>15.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3160,10 +3250,10 @@
                   <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>33.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3586,10 +3676,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3703,10 +3793,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4042,13 +4132,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4165,10 +4255,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6686,10 +6776,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -6955,8 +7041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AJ90"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:H2"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6977,7 +7063,7 @@
     <row r="1" spans="2:31" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:31" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="121" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="C2" s="121"/>
       <c r="D2" s="121"/>
@@ -6988,14 +7074,14 @@
     </row>
     <row r="3" spans="2:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="122" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="F3" s="122"/>
       <c r="G3" s="122"/>
@@ -7012,7 +7098,7 @@
     </row>
     <row r="5" spans="2:31" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -7021,34 +7107,34 @@
       <c r="G5" s="29"/>
       <c r="H5" s="60" t="str">
         <f>IF(L44=0,CONCATENATE(AE12, " totalisant ", AE15, " de travail estimé."),CONCATENATE("Attention, il reste " &amp; L45 &amp; " à remplir."))</f>
-        <v>4 tâches ont été définies totalisant 12 heures et 30 minutes de travail estimé.</v>
+        <v>24 tâches ont été définies totalisant 52 heures et 15 minutes de travail estimé.</v>
       </c>
     </row>
     <row r="6" spans="2:31" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="117" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="116" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="E7" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="118" t="s">
+      <c r="F7" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="118" t="s">
+      <c r="G7" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="118" t="s">
+      <c r="H7" s="120" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="118" t="s">
+      <c r="T7" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="H7" s="120" t="s">
-        <v>11</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
@@ -7056,13 +7142,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>12</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>14</v>
       </c>
       <c r="F8" s="14">
         <v>1</v>
@@ -7071,7 +7157,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L8" s="3" t="b">
         <f>AND(NOT(ISBLANK($C8)),LEN(D8)=0)</f>
@@ -7094,7 +7180,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="S8" s="23">
         <v>233</v>
@@ -7104,10 +7190,10 @@
       </c>
       <c r="U8" s="3">
         <f>MAX(B8:B42)</f>
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="W8" s="3">
         <v>1</v>
@@ -7120,7 +7206,7 @@
         <v>0.25</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AA8" s="3">
         <v>1</v>
@@ -7130,11 +7216,11 @@
       </c>
       <c r="AC8" s="4">
         <f>COUNTA(C8:C43)</f>
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="AD8" s="9">
         <f>SUM(G8:G43)</f>
-        <v>0.5208333333333337</v>
+        <v>2.1770833333333344</v>
       </c>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
@@ -7143,13 +7229,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D9" s="16">
         <v>1</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F9" s="16">
         <v>1</v>
@@ -7158,7 +7244,7 @@
         <v>0.25</v>
       </c>
       <c r="H9" s="41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L9" s="3" t="b">
         <f t="shared" ref="L9:L42" si="0">AND(NOT(ISBLANK($C9)),LEN(D9)=0)</f>
@@ -7181,7 +7267,7 @@
         <v>0</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="S9" s="23">
         <v>238</v>
@@ -7190,7 +7276,7 @@
         <v>2</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="W9" s="3">
         <v>2</v>
@@ -7199,7 +7285,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AA9" s="3">
         <v>2</v>
@@ -7209,7 +7295,7 @@
       </c>
       <c r="AD9" s="10">
         <f>AD8</f>
-        <v>0.5208333333333337</v>
+        <v>2.1770833333333344</v>
       </c>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
@@ -7218,13 +7304,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="18">
         <v>2</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F10" s="18">
         <v>2</v>
@@ -7233,7 +7319,7 @@
         <v>0.22916666666666699</v>
       </c>
       <c r="H10" s="42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L10" s="3" t="b">
         <f t="shared" si="0"/>
@@ -7256,7 +7342,7 @@
         <v>0</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S10" s="23">
         <v>243</v>
@@ -7271,7 +7357,7 @@
         <v>2.0833333333333301E-2</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AA10" s="3">
         <v>3</v>
@@ -7281,7 +7367,7 @@
       </c>
       <c r="AD10" s="63">
         <f>DAY(AD8)*24+HOUR(AD8)</f>
-        <v>12</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
@@ -7290,13 +7376,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="16">
         <v>3</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11" s="16">
         <v>2</v>
@@ -7305,7 +7391,7 @@
         <v>3.125E-2</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L11" s="3" t="b">
         <f t="shared" si="0"/>
@@ -7340,20 +7426,32 @@
       </c>
       <c r="AD11" s="4">
         <f>MINUTE(AD8)</f>
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B12" s="44" t="str">
+      <c r="B12" s="44">
         <f t="shared" ref="B12:B42" si="5">IF(LEN(C12)&lt;&gt;0,IF(OR(LEN(B11)=0,B11="^"),"^",B11+1),"")</f>
-        <v/>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="42"/>
+        <v>5</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="19">
+        <v>4</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="18">
+        <v>3</v>
+      </c>
+      <c r="G12" s="32">
+        <v>0.125</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="L12" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7375,7 +7473,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="S12" s="23">
         <v>212</v>
@@ -7390,28 +7488,40 @@
         <v>0.2</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AD12" s="4">
         <f>AC8</f>
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="AE12" s="4" t="str">
         <f>AD12 &amp; " " &amp; AC12 &amp; IF(AD12 &gt; 1, "s ont été définies", " a été définie")</f>
-        <v>4 tâches ont été définies</v>
+        <v>24 tâches ont été définies</v>
       </c>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="45" t="str">
+      <c r="B13" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="41"/>
+        <v>6</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="16">
+        <v>5</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="31">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>18</v>
+      </c>
       <c r="L13" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7433,7 +7543,7 @@
         <v>0</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="S13" s="23">
         <v>222</v>
@@ -7448,28 +7558,40 @@
         <v>0.25</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AD13" s="4">
         <f>AD10</f>
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="AE13" s="4" t="str">
         <f>AD13 &amp; " " &amp; AC13 &amp; IF(AD13 &gt; 1, "s", "")</f>
-        <v>12 heures</v>
+        <v>52 heures</v>
       </c>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B14" s="44" t="str">
+      <c r="B14" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="42"/>
+        <v>7</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="19">
+        <v>6</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="18">
+        <v>1</v>
+      </c>
+      <c r="G14" s="32">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H14" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="L14" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7491,7 +7613,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S14" s="23">
         <v>232</v>
@@ -7506,28 +7628,40 @@
         <v>0.3</v>
       </c>
       <c r="AC14" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="AD14" s="4">
         <f>AD11</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AE14" s="4" t="str">
         <f>AD14 &amp; " " &amp; AC14 &amp; IF(AD14 &gt; 1, "s", "")</f>
-        <v>30 minutes</v>
+        <v>15 minutes</v>
       </c>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B15" s="45" t="str">
+      <c r="B15" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="41"/>
+        <v>8</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="16">
+        <v>7</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="16">
+        <v>2</v>
+      </c>
+      <c r="G15" s="31">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>18</v>
+      </c>
       <c r="L15" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7559,20 +7693,32 @@
       </c>
       <c r="AE15" s="4" t="str">
         <f>IF(AD13&gt;0,IF(AD14&gt;0,AE13&amp;" et "&amp;AE14,AE13),AE14)</f>
-        <v>12 heures et 30 minutes</v>
+        <v>52 heures et 15 minutes</v>
       </c>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B16" s="44" t="str">
+      <c r="B16" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="42"/>
+        <v>9</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="18">
+        <v>8</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="18">
+        <v>1</v>
+      </c>
+      <c r="G16" s="32">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H16" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="L16" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7594,7 +7740,7 @@
         <v>0</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="S16" s="23">
         <v>58</v>
@@ -7610,16 +7756,28 @@
       </c>
     </row>
     <row r="17" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B17" s="45" t="str">
+      <c r="B17" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="41"/>
+        <v>10</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="16">
+        <v>10</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="16">
+        <v>2</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0.125</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>18</v>
+      </c>
       <c r="L17" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7641,7 +7799,7 @@
         <v>0</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="S17" s="23">
         <v>82</v>
@@ -7656,7 +7814,7 @@
         <v>0.45</v>
       </c>
       <c r="AC17" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="AD17" s="4">
         <f t="array" ref="AD17">SUM(($H$8:$H$42=$AC17)*$G$8:$G$42)</f>
@@ -7684,16 +7842,28 @@
       </c>
     </row>
     <row r="18" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B18" s="44" t="str">
+      <c r="B18" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="42"/>
+        <v>11</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="18">
+        <v>11</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="18">
+        <v>3</v>
+      </c>
+      <c r="G18" s="32">
+        <v>0.125</v>
+      </c>
+      <c r="H18" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="L18" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7715,7 +7885,7 @@
         <v>0</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S18" s="23">
         <v>106</v>
@@ -7730,44 +7900,56 @@
         <v>0.5</v>
       </c>
       <c r="AC18" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AD18" s="4">
         <f t="array" ref="AD18">SUM(($H$8:$H$42=$AC18)*$G$8:$G$42)</f>
-        <v>0</v>
+        <v>0.65625000000000011</v>
       </c>
       <c r="AE18" s="4">
         <f>AD18 * 24*60</f>
-        <v>0</v>
+        <v>945.00000000000023</v>
       </c>
       <c r="AF18" s="4">
         <f t="shared" ref="AF18:AF19" si="6">DAY(AD18)*24+HOUR(AD18)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AG18" s="4">
         <f t="shared" ref="AG18:AG19" si="7">MINUTE(AD18)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AH18" s="4" t="str">
         <f t="shared" ref="AH18:AH19" si="8">AF18&amp;"h"&amp;TEXT(AG18,"00")</f>
-        <v>0h00</v>
+        <v>15h45</v>
       </c>
       <c r="AJ18" s="4">
         <f>COUNTIF($H$8:$H$42,AC18)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B19" s="45" t="str">
+      <c r="B19" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="41"/>
+        <v>12</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="16">
+        <v>15</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="16">
+        <v>1</v>
+      </c>
+      <c r="G19" s="31">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H19" s="41" t="s">
+        <v>21</v>
+      </c>
       <c r="L19" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7798,19 +7980,19 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="AC19" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="AD19" s="4">
         <f t="array" ref="AD19">SUM(($H$8:$H$42=$AC19)*$G$8:$G$42)</f>
-        <v>0</v>
+        <v>1.0000000000000004</v>
       </c>
       <c r="AE19" s="4">
         <f>AD19 * 24*60</f>
-        <v>0</v>
+        <v>1440.0000000000007</v>
       </c>
       <c r="AF19" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AG19" s="4">
         <f t="shared" si="7"/>
@@ -7818,24 +8000,36 @@
       </c>
       <c r="AH19" s="4" t="str">
         <f t="shared" si="8"/>
-        <v>0h00</v>
+        <v>24h00</v>
       </c>
       <c r="AJ19" s="4">
         <f>COUNTIF($H$8:$H$42,AC19)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B20" s="44" t="str">
+      <c r="B20" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="42"/>
+        <v>13</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="19">
+        <v>20</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="18">
+        <v>3</v>
+      </c>
+      <c r="G20" s="32">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H20" s="42" t="s">
+        <v>21</v>
+      </c>
       <c r="L20" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7868,16 +8062,28 @@
       </c>
     </row>
     <row r="21" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B21" s="45" t="str">
+      <c r="B21" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="41"/>
+        <v>14</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="16">
+        <v>18</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="16">
+        <v>3</v>
+      </c>
+      <c r="G21" s="31">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H21" s="41" t="s">
+        <v>21</v>
+      </c>
       <c r="L21" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7909,36 +8115,48 @@
       </c>
       <c r="AD21" s="4">
         <f>SUM(AD17:AD19)</f>
-        <v>0.5208333333333337</v>
+        <v>2.1770833333333344</v>
       </c>
       <c r="AE21" s="4">
         <f t="shared" ref="AE21" si="9">AD21 * 24*60</f>
-        <v>750.00000000000057</v>
+        <v>3135.0000000000018</v>
       </c>
       <c r="AF21" s="4">
         <f t="shared" ref="AF21" si="10">DAY(AD21)*24+HOUR(AD21)</f>
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" ref="AG21" si="11">MINUTE(AD21)</f>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AH21" s="4" t="str">
         <f t="shared" ref="AH21" si="12">AF21&amp;"h"&amp;TEXT(AG21,"00")</f>
-        <v>12h30</v>
+        <v>52h15</v>
       </c>
     </row>
     <row r="22" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B22" s="44" t="str">
+      <c r="B22" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="42"/>
+        <v>15</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="18">
+        <v>9</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="18">
+        <v>1</v>
+      </c>
+      <c r="G22" s="32">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H22" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="L22" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7970,16 +8188,28 @@
       </c>
     </row>
     <row r="23" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B23" s="45" t="str">
+      <c r="B23" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="41"/>
+        <v>16</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="16">
+        <v>20</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="16">
+        <v>3</v>
+      </c>
+      <c r="G23" s="31">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="H23" s="41" t="s">
+        <v>21</v>
+      </c>
       <c r="L23" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8011,16 +8241,28 @@
       </c>
     </row>
     <row r="24" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B24" s="44" t="str">
+      <c r="B24" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="42"/>
+        <v>17</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="19">
+        <v>20</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="18">
+        <v>3</v>
+      </c>
+      <c r="G24" s="32">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="H24" s="42" t="s">
+        <v>21</v>
+      </c>
       <c r="L24" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8052,16 +8294,28 @@
       </c>
     </row>
     <row r="25" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B25" s="45" t="str">
+      <c r="B25" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="41"/>
+        <v>18</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="16">
+        <v>3</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="16">
+        <v>3</v>
+      </c>
+      <c r="G25" s="31">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="H25" s="41" t="s">
+        <v>21</v>
+      </c>
       <c r="L25" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8093,16 +8347,28 @@
       </c>
     </row>
     <row r="26" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="str">
+      <c r="B26" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="42"/>
+        <v>19</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="19">
+        <v>14</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="18">
+        <v>3</v>
+      </c>
+      <c r="G26" s="32">
+        <v>0.125</v>
+      </c>
+      <c r="H26" s="42" t="s">
+        <v>21</v>
+      </c>
       <c r="L26" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8134,16 +8400,28 @@
       </c>
     </row>
     <row r="27" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B27" s="45" t="str">
+      <c r="B27" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="41"/>
+        <v>20</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="16">
+        <v>13</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="16">
+        <v>2</v>
+      </c>
+      <c r="G27" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H27" s="41" t="s">
+        <v>18</v>
+      </c>
       <c r="L27" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8175,16 +8453,28 @@
       </c>
     </row>
     <row r="28" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="str">
+      <c r="B28" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="42"/>
+        <v>21</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="18">
+        <v>12</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="18">
+        <v>2</v>
+      </c>
+      <c r="G28" s="32">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H28" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="L28" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8216,16 +8506,28 @@
       </c>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B29" s="45" t="str">
+      <c r="B29" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="41"/>
+        <v>22</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="16">
+        <v>17</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="16">
+        <v>1</v>
+      </c>
+      <c r="G29" s="31">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H29" s="41" t="s">
+        <v>21</v>
+      </c>
       <c r="L29" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8254,16 +8556,28 @@
       </c>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B30" s="44" t="str">
+      <c r="B30" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="42"/>
+        <v>23</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="19">
+        <v>16</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="18">
+        <v>1</v>
+      </c>
+      <c r="G30" s="32">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H30" s="42" t="s">
+        <v>21</v>
+      </c>
       <c r="L30" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8292,16 +8606,28 @@
       </c>
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B31" s="45" t="str">
+      <c r="B31" s="45">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="41"/>
+        <v>24</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="16">
+        <v>19</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="16">
+        <v>2</v>
+      </c>
+      <c r="G31" s="31">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H31" s="41" t="s">
+        <v>21</v>
+      </c>
       <c r="L31" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -9183,7 +9509,7 @@
       <formula>LEN($B12)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations xWindow="818" yWindow="682" count="7">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nom de tâche trop long" error="Le nom de votre tâche doit être court. _x000a_Un maximum de 72 caractères est mis à votre disposition._x000a_Pour plus de détail, veuillez faire l'ajout de commentaires." promptTitle="Nom de la tâche" prompt="_x000a_Veuillez saisir le nom de la tâche._x000a__x000a_Lorsque pertinent, n'oubliez pas d'ajouter une description de votre tâche sous forme de commentaire." sqref="C8:C42" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>72</formula2>
@@ -9282,8 +9608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:W56"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9304,7 +9630,7 @@
     <row r="2" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="123" t="str">
         <f>'Sprint 1 - Planification'!B2:H2</f>
-        <v>Nom du projet super cool que vous faites!</v>
+        <v>UnoJS</v>
       </c>
       <c r="C2" s="123"/>
       <c r="D2" s="123"/>
@@ -9314,7 +9640,7 @@
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="33"/>
@@ -9332,7 +9658,7 @@
     </row>
     <row r="5" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
@@ -9346,22 +9672,22 @@
     <row r="6" spans="2:23" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7" s="117" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="116" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="118" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="117" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="118" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="120" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" s="117" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="118" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="120" t="s">
-        <v>32</v>
       </c>
       <c r="K7" s="7"/>
     </row>
@@ -9385,7 +9711,7 @@
         <v>0.95</v>
       </c>
       <c r="G8" s="105" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K8" s="3" t="b">
         <f>AND($D8="Sprint 1",ISBLANK(E8))</f>
@@ -9400,7 +9726,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Q8" s="61">
         <f t="array" ref="Q8">SUM(($D$8:$D$42=$P8)*$E$8:$E$42)</f>
@@ -9448,7 +9774,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="Q9" s="61">
         <f t="array" ref="Q9">SUM(($D$8:$D$42=$P9)*$E$8:$E$42)</f>
@@ -9496,7 +9822,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q10" s="61">
         <f t="array" ref="Q10">SUM(($D$8:$D$42=$P10)*$E$8:$E$42)</f>
@@ -9552,17 +9878,17 @@
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B12" s="53" t="str">
+      <c r="B12" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B12)&lt;&gt;0,'Sprint 1 - Planification'!B12,"")</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="C12" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C12)&lt;&gt;0,'Sprint 1 - Planification'!C12,"")</f>
-        <v/>
+        <v>Creer une classe mère carte</v>
       </c>
       <c r="D12" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H12)&lt;&gt;0,'Sprint 1 - Planification'!H12,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E12" s="112"/>
       <c r="F12" s="110"/>
@@ -9581,7 +9907,7 @@
       </c>
       <c r="P12" s="8"/>
       <c r="S12" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="T12" s="63">
         <f>T10</f>
@@ -9593,17 +9919,17 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="50" t="str">
+      <c r="B13" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B13)&lt;&gt;0,'Sprint 1 - Planification'!B13,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="C13" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C13)&lt;&gt;0,'Sprint 1 - Planification'!C13,"")</f>
-        <v/>
+        <v>Creer une classe deck</v>
       </c>
       <c r="D13" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H13)&lt;&gt;0,'Sprint 1 - Planification'!H13,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E13" s="106"/>
       <c r="F13" s="107"/>
@@ -9622,7 +9948,7 @@
       </c>
       <c r="P13" s="8"/>
       <c r="S13" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="T13" s="4">
         <f>T11</f>
@@ -9634,17 +9960,17 @@
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B14" s="53" t="str">
+      <c r="B14" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B14)&lt;&gt;0,'Sprint 1 - Planification'!B14,"")</f>
-        <v/>
+        <v>7</v>
       </c>
       <c r="C14" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C14)&lt;&gt;0,'Sprint 1 - Planification'!C14,"")</f>
-        <v/>
+        <v>creer une classe hand</v>
       </c>
       <c r="D14" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H14)&lt;&gt;0,'Sprint 1 - Planification'!H14,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E14" s="112"/>
       <c r="F14" s="110"/>
@@ -9672,17 +9998,17 @@
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="50" t="str">
+      <c r="B15" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B15)&lt;&gt;0,'Sprint 1 - Planification'!B15,"")</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="C15" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C15)&lt;&gt;0,'Sprint 1 - Planification'!C15,"")</f>
-        <v/>
+        <v>creer une classe joueur</v>
       </c>
       <c r="D15" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H15)&lt;&gt;0,'Sprint 1 - Planification'!H15,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E15" s="106"/>
       <c r="F15" s="107"/>
@@ -9710,17 +10036,17 @@
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="53" t="str">
+      <c r="B16" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B16)&lt;&gt;0,'Sprint 1 - Planification'!B16,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="C16" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C16)&lt;&gt;0,'Sprint 1 - Planification'!C16,"")</f>
-        <v/>
+        <v>creer une classe table</v>
       </c>
       <c r="D16" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H16)&lt;&gt;0,'Sprint 1 - Planification'!H16,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E16" s="109"/>
       <c r="F16" s="110"/>
@@ -9740,17 +10066,17 @@
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="50" t="str">
+      <c r="B17" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B17)&lt;&gt;0,'Sprint 1 - Planification'!B17,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="C17" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C17)&lt;&gt;0,'Sprint 1 - Planification'!C17,"")</f>
-        <v/>
+        <v>creer une variable globale jeu</v>
       </c>
       <c r="D17" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H17)&lt;&gt;0,'Sprint 1 - Planification'!H17,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E17" s="106"/>
       <c r="F17" s="107"/>
@@ -9770,17 +10096,17 @@
       <c r="P17" s="8"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="53" t="str">
+      <c r="B18" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B18)&lt;&gt;0,'Sprint 1 - Planification'!B18,"")</f>
-        <v/>
+        <v>11</v>
       </c>
       <c r="C18" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C18)&lt;&gt;0,'Sprint 1 - Planification'!C18,"")</f>
-        <v/>
+        <v>creer une classe règles</v>
       </c>
       <c r="D18" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H18)&lt;&gt;0,'Sprint 1 - Planification'!H18,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E18" s="112"/>
       <c r="F18" s="110"/>
@@ -9800,17 +10126,17 @@
       <c r="P18" s="8"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="50" t="str">
+      <c r="B19" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B19)&lt;&gt;0,'Sprint 1 - Planification'!B19,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="C19" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C19)&lt;&gt;0,'Sprint 1 - Planification'!C19,"")</f>
-        <v/>
+        <v>creer un lobby</v>
       </c>
       <c r="D19" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H19)&lt;&gt;0,'Sprint 1 - Planification'!H19,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E19" s="106"/>
       <c r="F19" s="107"/>
@@ -9830,17 +10156,17 @@
       <c r="P19" s="8"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="53" t="str">
+      <c r="B20" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B20)&lt;&gt;0,'Sprint 1 - Planification'!B20,"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C20" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C20)&lt;&gt;0,'Sprint 1 - Planification'!C20,"")</f>
-        <v/>
+        <v>créer un menu</v>
       </c>
       <c r="D20" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H20)&lt;&gt;0,'Sprint 1 - Planification'!H20,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E20" s="112"/>
       <c r="F20" s="110"/>
@@ -9860,17 +10186,17 @@
       <c r="P20" s="8"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="50" t="str">
+      <c r="B21" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B21)&lt;&gt;0,'Sprint 1 - Planification'!B21,"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C21" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C21)&lt;&gt;0,'Sprint 1 - Planification'!C21,"")</f>
-        <v/>
+        <v>créer mécanique UNO</v>
       </c>
       <c r="D21" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H21)&lt;&gt;0,'Sprint 1 - Planification'!H21,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E21" s="106"/>
       <c r="F21" s="107"/>
@@ -9890,17 +10216,17 @@
       <c r="P21" s="8"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="53" t="str">
+      <c r="B22" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B22)&lt;&gt;0,'Sprint 1 - Planification'!B22,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C22" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C22)&lt;&gt;0,'Sprint 1 - Planification'!C22,"")</f>
-        <v/>
+        <v>implémenter un random des cartes</v>
       </c>
       <c r="D22" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H22)&lt;&gt;0,'Sprint 1 - Planification'!H22,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E22" s="109"/>
       <c r="F22" s="110"/>
@@ -9920,17 +10246,17 @@
       <c r="P22" s="8"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="50" t="str">
+      <c r="B23" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B23)&lt;&gt;0,'Sprint 1 - Planification'!B23,"")</f>
-        <v/>
+        <v>16</v>
       </c>
       <c r="C23" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C23)&lt;&gt;0,'Sprint 1 - Planification'!C23,"")</f>
-        <v/>
+        <v>créer un algorithme d'affichage des joueurs</v>
       </c>
       <c r="D23" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H23)&lt;&gt;0,'Sprint 1 - Planification'!H23,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E23" s="106"/>
       <c r="F23" s="107"/>
@@ -9950,17 +10276,17 @@
       <c r="P23" s="8"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="53" t="str">
+      <c r="B24" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B24)&lt;&gt;0,'Sprint 1 - Planification'!B24,"")</f>
-        <v/>
+        <v>17</v>
       </c>
       <c r="C24" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C24)&lt;&gt;0,'Sprint 1 - Planification'!C24,"")</f>
-        <v/>
+        <v>Créer le code reliant client-serveur</v>
       </c>
       <c r="D24" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H24)&lt;&gt;0,'Sprint 1 - Planification'!H24,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E24" s="112"/>
       <c r="F24" s="110"/>
@@ -9980,17 +10306,17 @@
       <c r="P24" s="8"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="50" t="str">
+      <c r="B25" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B25)&lt;&gt;0,'Sprint 1 - Planification'!B25,"")</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="C25" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C25)&lt;&gt;0,'Sprint 1 - Planification'!C25,"")</f>
-        <v/>
+        <v>Se procurer un serveur</v>
       </c>
       <c r="D25" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H25)&lt;&gt;0,'Sprint 1 - Planification'!H25,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E25" s="106"/>
       <c r="F25" s="107"/>
@@ -10010,17 +10336,17 @@
       <c r="P25" s="8"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="53" t="str">
+      <c r="B26" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B26)&lt;&gt;0,'Sprint 1 - Planification'!B26,"")</f>
-        <v/>
+        <v>19</v>
       </c>
       <c r="C26" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v/>
+        <v>Créer un menu d'options</v>
       </c>
       <c r="D26" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E26" s="112"/>
       <c r="F26" s="110"/>
@@ -10040,17 +10366,17 @@
       <c r="P26" s="8"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="50" t="str">
+      <c r="B27" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B27)&lt;&gt;0,'Sprint 1 - Planification'!B27,"")</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="C27" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C27)&lt;&gt;0,'Sprint 1 - Planification'!C27,"")</f>
-        <v/>
+        <v>Créer un UI de gameplay</v>
       </c>
       <c r="D27" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H27)&lt;&gt;0,'Sprint 1 - Planification'!H27,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E27" s="106"/>
       <c r="F27" s="107"/>
@@ -10070,17 +10396,17 @@
       <c r="P27" s="8"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="53" t="str">
+      <c r="B28" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B28)&lt;&gt;0,'Sprint 1 - Planification'!B28,"")</f>
-        <v/>
+        <v>21</v>
       </c>
       <c r="C28" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C28)&lt;&gt;0,'Sprint 1 - Planification'!C28,"")</f>
-        <v/>
+        <v>Créer un UI pour la carte</v>
       </c>
       <c r="D28" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H28)&lt;&gt;0,'Sprint 1 - Planification'!H28,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E28" s="109"/>
       <c r="F28" s="110"/>
@@ -10100,17 +10426,17 @@
       <c r="P28" s="8"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="50" t="str">
+      <c r="B29" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B29)&lt;&gt;0,'Sprint 1 - Planification'!B29,"")</f>
-        <v/>
+        <v>22</v>
       </c>
       <c r="C29" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C29)&lt;&gt;0,'Sprint 1 - Planification'!C29,"")</f>
-        <v/>
+        <v>Créer l'animation des cartes</v>
       </c>
       <c r="D29" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H29)&lt;&gt;0,'Sprint 1 - Planification'!H29,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E29" s="106"/>
       <c r="F29" s="107"/>
@@ -10130,17 +10456,17 @@
       <c r="P29" s="8"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="53" t="str">
+      <c r="B30" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B30)&lt;&gt;0,'Sprint 1 - Planification'!B30,"")</f>
-        <v/>
+        <v>23</v>
       </c>
       <c r="C30" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C30)&lt;&gt;0,'Sprint 1 - Planification'!C30,"")</f>
-        <v/>
+        <v>Créer un UI pour le wild card</v>
       </c>
       <c r="D30" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H30)&lt;&gt;0,'Sprint 1 - Planification'!H30,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E30" s="112"/>
       <c r="F30" s="110"/>
@@ -10160,17 +10486,17 @@
       <c r="P30" s="8"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="50" t="str">
+      <c r="B31" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B31)&lt;&gt;0,'Sprint 1 - Planification'!B31,"")</f>
-        <v/>
+        <v>24</v>
       </c>
       <c r="C31" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C31)&lt;&gt;0,'Sprint 1 - Planification'!C31,"")</f>
-        <v/>
+        <v>créer un système de point</v>
       </c>
       <c r="D31" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H31)&lt;&gt;0,'Sprint 1 - Planification'!H31,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E31" s="106"/>
       <c r="F31" s="107"/>
@@ -10728,7 +11054,7 @@
     <row r="2" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="123" t="str">
         <f>'Sprint 1 - Planification'!B2:H2</f>
-        <v>Nom du projet super cool que vous faites!</v>
+        <v>UnoJS</v>
       </c>
       <c r="C2" s="123"/>
       <c r="D2" s="123"/>
@@ -10740,7 +11066,7 @@
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="33"/>
@@ -10762,7 +11088,7 @@
     </row>
     <row r="5" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
@@ -10772,32 +11098,32 @@
       <c r="H5" s="35"/>
       <c r="I5" s="64" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 2 champs à remplir!</v>
+        <v>Attention, il reste 1 champ à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="131" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="129" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="127" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="125" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" s="126"/>
       <c r="G7" s="131" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H7" s="133" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I7" s="135" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M7" s="7"/>
     </row>
@@ -10806,10 +11132,10 @@
       <c r="C8" s="130"/>
       <c r="D8" s="128"/>
       <c r="E8" s="119" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F8" s="119" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G8" s="132"/>
       <c r="H8" s="134"/>
@@ -10837,16 +11163,20 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F8),"",'Sprint 1 - Bilan'!F8)</f>
         <v>0.95</v>
       </c>
-      <c r="G9" s="103"/>
-      <c r="H9" s="104"/>
+      <c r="G9" s="103">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H9" s="104">
+        <v>1</v>
+      </c>
       <c r="I9" s="105"/>
       <c r="M9" s="3" t="b">
         <f>OR(AND(NOT(P9),LEN($G9)=0),AND(LEN($H9)&gt;0,LEN($G9)=0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="3" t="b">
         <f>AND(NOT($P9),LEN($H9)=0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" s="3" t="b">
         <f>AND($D9&lt;&gt;"Sprint 3",NOT(ISBLANK($H9)),$H9&lt;100%,ISBLANK($I9))</f>
@@ -10854,22 +11184,22 @@
       </c>
       <c r="P9" s="3" t="b">
         <f>IF(OR(LEN($D9)=0,$D9="Sprint 3"),TRUE,IF(COUNTA($F9)=0,IF(LEN($H9)=0,FALSE,$H9=100%),IF($F9=100%,TRUE,IF(LEN($H9)=0,FALSE,$H9=100%))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="S9" s="61">
         <f t="array" ref="S9">SUM(($D$9:$D$43=$R9)*$G$9:$G$43)</f>
-        <v>0</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="T9" s="62">
         <f>S9*24*60</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="V9" s="9">
         <f>SUM(G9:G43)</f>
-        <v>0</v>
+        <v>1.0833333333333326</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
@@ -10913,19 +11243,19 @@
         <v>1</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="S10" s="61">
         <f t="array" ref="S10">SUM(($D$9:$D$43=$R10)*$G$9:$G$43)</f>
-        <v>0</v>
+        <v>1.0729166666666659</v>
       </c>
       <c r="T10" s="62">
         <f t="shared" ref="T10:T11" si="4">S10*24*60</f>
-        <v>0</v>
+        <v>1544.9999999999986</v>
       </c>
       <c r="V10" s="10">
         <f>V9</f>
-        <v>0</v>
+        <v>1.0833333333333326</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -10969,7 +11299,7 @@
         <v>1</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S11" s="61">
         <f t="array" ref="S11">SUM(($D$9:$D$43=$R11)*$G$9:$G$43)</f>
@@ -10981,7 +11311,7 @@
       </c>
       <c r="V11" s="63">
         <f>DAY(V9)*24+HOUR(V9)</f>
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -11032,17 +11362,17 @@
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="53" t="str">
+      <c r="B13" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B12)&lt;&gt;0,'Sprint 1 - Planification'!B12,"")</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="C13" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C12)&lt;&gt;0,'Sprint 1 - Planification'!C12,"")</f>
-        <v/>
+        <v>Creer une classe mère carte</v>
       </c>
       <c r="D13" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H12)&lt;&gt;0,'Sprint 1 - Planification'!H12,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E13" s="69" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E12),"",'Sprint 1 - Bilan'!E12)</f>
@@ -11052,8 +11382,12 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F12),"",'Sprint 1 - Bilan'!F12)</f>
         <v/>
       </c>
-      <c r="G13" s="112"/>
-      <c r="H13" s="110"/>
+      <c r="G13" s="112">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H13" s="110">
+        <v>1</v>
+      </c>
       <c r="I13" s="111"/>
       <c r="M13" s="3" t="b">
         <f t="shared" si="0"/>
@@ -11073,29 +11407,29 @@
       </c>
       <c r="R13" s="8"/>
       <c r="U13" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="V13" s="63">
         <f>V11</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="W13" s="4" t="str">
         <f>V13 &amp; " " &amp; U13 &amp; IF(V13 &gt; 1, "s", "")</f>
-        <v>0 heure</v>
+        <v>26 heures</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B14" s="50" t="str">
+      <c r="B14" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B13)&lt;&gt;0,'Sprint 1 - Planification'!B13,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="C14" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C13)&lt;&gt;0,'Sprint 1 - Planification'!C13,"")</f>
-        <v/>
+        <v>Creer une classe deck</v>
       </c>
       <c r="D14" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H13)&lt;&gt;0,'Sprint 1 - Planification'!H13,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E14" s="67" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E13),"",'Sprint 1 - Bilan'!E13)</f>
@@ -11105,8 +11439,12 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F13),"",'Sprint 1 - Bilan'!F13)</f>
         <v/>
       </c>
-      <c r="G14" s="106"/>
-      <c r="H14" s="107"/>
+      <c r="G14" s="106">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H14" s="107">
+        <v>1</v>
+      </c>
       <c r="I14" s="108"/>
       <c r="M14" s="3" t="b">
         <f t="shared" si="0"/>
@@ -11126,7 +11464,7 @@
       </c>
       <c r="R14" s="8"/>
       <c r="U14" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="V14" s="4">
         <f>V12</f>
@@ -11138,17 +11476,17 @@
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="53" t="str">
+      <c r="B15" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B14)&lt;&gt;0,'Sprint 1 - Planification'!B14,"")</f>
-        <v/>
+        <v>7</v>
       </c>
       <c r="C15" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C14)&lt;&gt;0,'Sprint 1 - Planification'!C14,"")</f>
-        <v/>
+        <v>creer une classe hand</v>
       </c>
       <c r="D15" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H14)&lt;&gt;0,'Sprint 1 - Planification'!H14,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E15" s="69" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E14),"",'Sprint 1 - Bilan'!E14)</f>
@@ -11158,8 +11496,12 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F14),"",'Sprint 1 - Bilan'!F14)</f>
         <v/>
       </c>
-      <c r="G15" s="112"/>
-      <c r="H15" s="110"/>
+      <c r="G15" s="112">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H15" s="110">
+        <v>1</v>
+      </c>
       <c r="I15" s="111"/>
       <c r="M15" s="3" t="b">
         <f t="shared" si="0"/>
@@ -11180,25 +11522,25 @@
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
         <f>IF(V13&gt;0,IF(V14&gt;0,W13&amp;" et "&amp;W14,W13),W14)</f>
-        <v>0 minute</v>
+        <v>26 heures</v>
       </c>
       <c r="Y15" s="4" t="str">
         <f>V13&amp;"h"&amp;TEXT(V14,"00")</f>
-        <v>0h00</v>
+        <v>26h00</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B16" s="50" t="str">
+      <c r="B16" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B15)&lt;&gt;0,'Sprint 1 - Planification'!B15,"")</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="C16" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C15)&lt;&gt;0,'Sprint 1 - Planification'!C15,"")</f>
-        <v/>
+        <v>creer une classe joueur</v>
       </c>
       <c r="D16" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H15)&lt;&gt;0,'Sprint 1 - Planification'!H15,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E16" s="67" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E15),"",'Sprint 1 - Bilan'!E15)</f>
@@ -11208,8 +11550,12 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F15),"",'Sprint 1 - Bilan'!F15)</f>
         <v/>
       </c>
-      <c r="G16" s="106"/>
-      <c r="H16" s="107"/>
+      <c r="G16" s="106">
+        <v>0.125</v>
+      </c>
+      <c r="H16" s="107">
+        <v>0.9</v>
+      </c>
       <c r="I16" s="108"/>
       <c r="M16" s="3" t="b">
         <f t="shared" si="0"/>
@@ -11221,34 +11567,34 @@
       </c>
       <c r="O16" s="3" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche est en retard!",CONCATENATE(V16," tâches sont en retard!")))</f>
-        <v>Une tâche est en retard!</v>
+        <v>3 tâches sont en retard!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="53" t="str">
+      <c r="B17" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B16)&lt;&gt;0,'Sprint 1 - Planification'!B16,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="C17" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C16)&lt;&gt;0,'Sprint 1 - Planification'!C16,"")</f>
-        <v/>
+        <v>creer une classe table</v>
       </c>
       <c r="D17" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H16)&lt;&gt;0,'Sprint 1 - Planification'!H16,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E17" s="68" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E16),"",'Sprint 1 - Bilan'!E16)</f>
@@ -11258,9 +11604,15 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F16),"",'Sprint 1 - Bilan'!F16)</f>
         <v/>
       </c>
-      <c r="G17" s="109"/>
-      <c r="H17" s="110"/>
-      <c r="I17" s="111"/>
+      <c r="G17" s="109">
+        <v>0.14583333333333301</v>
+      </c>
+      <c r="H17" s="110">
+        <v>0.8</v>
+      </c>
+      <c r="I17" s="111" t="s">
+        <v>98</v>
+      </c>
       <c r="M17" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -11275,22 +11627,22 @@
       </c>
       <c r="P17" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="8"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="50" t="str">
+      <c r="B18" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B17)&lt;&gt;0,'Sprint 1 - Planification'!B17,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="C18" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C17)&lt;&gt;0,'Sprint 1 - Planification'!C17,"")</f>
-        <v/>
+        <v>creer une variable globale jeu</v>
       </c>
       <c r="D18" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H17)&lt;&gt;0,'Sprint 1 - Planification'!H17,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E18" s="67" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E17),"",'Sprint 1 - Bilan'!E17)</f>
@@ -11300,8 +11652,12 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F17),"",'Sprint 1 - Bilan'!F17)</f>
         <v/>
       </c>
-      <c r="G18" s="106"/>
-      <c r="H18" s="107"/>
+      <c r="G18" s="106">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H18" s="107">
+        <v>1</v>
+      </c>
       <c r="I18" s="108"/>
       <c r="M18" s="3" t="b">
         <f t="shared" si="0"/>
@@ -11322,17 +11678,17 @@
       <c r="R18" s="8"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="53" t="str">
+      <c r="B19" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B18)&lt;&gt;0,'Sprint 1 - Planification'!B18,"")</f>
-        <v/>
+        <v>11</v>
       </c>
       <c r="C19" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C18)&lt;&gt;0,'Sprint 1 - Planification'!C18,"")</f>
-        <v/>
+        <v>creer une classe règles</v>
       </c>
       <c r="D19" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H18)&lt;&gt;0,'Sprint 1 - Planification'!H18,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E19" s="69" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E18),"",'Sprint 1 - Bilan'!E18)</f>
@@ -11342,9 +11698,15 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F18),"",'Sprint 1 - Bilan'!F18)</f>
         <v/>
       </c>
-      <c r="G19" s="112"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="111"/>
+      <c r="G19" s="112">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H19" s="110">
+        <v>0.7</v>
+      </c>
+      <c r="I19" s="111" t="s">
+        <v>96</v>
+      </c>
       <c r="K19" s="9"/>
       <c r="M19" s="3" t="b">
         <f t="shared" si="0"/>
@@ -11360,22 +11722,22 @@
       </c>
       <c r="P19" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" s="8"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="50" t="str">
+      <c r="B20" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B19)&lt;&gt;0,'Sprint 1 - Planification'!B19,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="C20" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C19)&lt;&gt;0,'Sprint 1 - Planification'!C19,"")</f>
-        <v/>
+        <v>creer un lobby</v>
       </c>
       <c r="D20" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H19)&lt;&gt;0,'Sprint 1 - Planification'!H19,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E20" s="67" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E19),"",'Sprint 1 - Bilan'!E19)</f>
@@ -11407,17 +11769,17 @@
       <c r="R20" s="8"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="53" t="str">
+      <c r="B21" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B20)&lt;&gt;0,'Sprint 1 - Planification'!B20,"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C21" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C20)&lt;&gt;0,'Sprint 1 - Planification'!C20,"")</f>
-        <v/>
+        <v>créer un menu</v>
       </c>
       <c r="D21" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H20)&lt;&gt;0,'Sprint 1 - Planification'!H20,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E21" s="69" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E20),"",'Sprint 1 - Bilan'!E20)</f>
@@ -11449,17 +11811,17 @@
       <c r="R21" s="8"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="50" t="str">
+      <c r="B22" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B21)&lt;&gt;0,'Sprint 1 - Planification'!B21,"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C22" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C21)&lt;&gt;0,'Sprint 1 - Planification'!C21,"")</f>
-        <v/>
+        <v>créer mécanique UNO</v>
       </c>
       <c r="D22" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H21)&lt;&gt;0,'Sprint 1 - Planification'!H21,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E22" s="67" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E21),"",'Sprint 1 - Bilan'!E21)</f>
@@ -11491,17 +11853,17 @@
       <c r="R22" s="8"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="53" t="str">
+      <c r="B23" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B22)&lt;&gt;0,'Sprint 1 - Planification'!B22,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C23" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C22)&lt;&gt;0,'Sprint 1 - Planification'!C22,"")</f>
-        <v/>
+        <v>implémenter un random des cartes</v>
       </c>
       <c r="D23" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H22)&lt;&gt;0,'Sprint 1 - Planification'!H22,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E23" s="68" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E22),"",'Sprint 1 - Bilan'!E22)</f>
@@ -11511,8 +11873,12 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F22),"",'Sprint 1 - Bilan'!F22)</f>
         <v/>
       </c>
-      <c r="G23" s="109"/>
-      <c r="H23" s="110"/>
+      <c r="G23" s="109">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="H23" s="110">
+        <v>1</v>
+      </c>
       <c r="I23" s="111"/>
       <c r="M23" s="3" t="b">
         <f t="shared" si="0"/>
@@ -11533,17 +11899,17 @@
       <c r="R23" s="8"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="50" t="str">
+      <c r="B24" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B23)&lt;&gt;0,'Sprint 1 - Planification'!B23,"")</f>
-        <v/>
+        <v>16</v>
       </c>
       <c r="C24" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C23)&lt;&gt;0,'Sprint 1 - Planification'!C23,"")</f>
-        <v/>
+        <v>créer un algorithme d'affichage des joueurs</v>
       </c>
       <c r="D24" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H23)&lt;&gt;0,'Sprint 1 - Planification'!H23,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E24" s="67" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E23),"",'Sprint 1 - Bilan'!E23)</f>
@@ -11575,17 +11941,17 @@
       <c r="R24" s="8"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="53" t="str">
+      <c r="B25" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B24)&lt;&gt;0,'Sprint 1 - Planification'!B24,"")</f>
-        <v/>
+        <v>17</v>
       </c>
       <c r="C25" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C24)&lt;&gt;0,'Sprint 1 - Planification'!C24,"")</f>
-        <v/>
+        <v>Créer le code reliant client-serveur</v>
       </c>
       <c r="D25" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H24)&lt;&gt;0,'Sprint 1 - Planification'!H24,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E25" s="69" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E24),"",'Sprint 1 - Bilan'!E24)</f>
@@ -11617,17 +11983,17 @@
       <c r="R25" s="8"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="str">
+      <c r="B26" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B25)&lt;&gt;0,'Sprint 1 - Planification'!B25,"")</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="C26" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C25)&lt;&gt;0,'Sprint 1 - Planification'!C25,"")</f>
-        <v/>
+        <v>Se procurer un serveur</v>
       </c>
       <c r="D26" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H25)&lt;&gt;0,'Sprint 1 - Planification'!H25,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E26" s="67" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E25),"",'Sprint 1 - Bilan'!E25)</f>
@@ -11659,17 +12025,17 @@
       <c r="R26" s="8"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="53" t="str">
+      <c r="B27" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B26)&lt;&gt;0,'Sprint 1 - Planification'!B26,"")</f>
-        <v/>
+        <v>19</v>
       </c>
       <c r="C27" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v/>
+        <v>Créer un menu d'options</v>
       </c>
       <c r="D27" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E27" s="69" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E26),"",'Sprint 1 - Bilan'!E26)</f>
@@ -11701,17 +12067,17 @@
       <c r="R27" s="8"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="50" t="str">
+      <c r="B28" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B27)&lt;&gt;0,'Sprint 1 - Planification'!B27,"")</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="C28" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C27)&lt;&gt;0,'Sprint 1 - Planification'!C27,"")</f>
-        <v/>
+        <v>Créer un UI de gameplay</v>
       </c>
       <c r="D28" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H27)&lt;&gt;0,'Sprint 1 - Planification'!H27,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E28" s="67" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E27),"",'Sprint 1 - Bilan'!E27)</f>
@@ -11721,8 +12087,12 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F27),"",'Sprint 1 - Bilan'!F27)</f>
         <v/>
       </c>
-      <c r="G28" s="106"/>
-      <c r="H28" s="107"/>
+      <c r="G28" s="106">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="H28" s="107">
+        <v>1</v>
+      </c>
       <c r="I28" s="108"/>
       <c r="M28" s="3" t="b">
         <f t="shared" si="0"/>
@@ -11743,17 +12113,17 @@
       <c r="R28" s="8"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="53" t="str">
+      <c r="B29" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B28)&lt;&gt;0,'Sprint 1 - Planification'!B28,"")</f>
-        <v/>
+        <v>21</v>
       </c>
       <c r="C29" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C28)&lt;&gt;0,'Sprint 1 - Planification'!C28,"")</f>
-        <v/>
+        <v>Créer un UI pour la carte</v>
       </c>
       <c r="D29" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H28)&lt;&gt;0,'Sprint 1 - Planification'!H28,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E29" s="68" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E28),"",'Sprint 1 - Bilan'!E28)</f>
@@ -11763,9 +12133,15 @@
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F28),"",'Sprint 1 - Bilan'!F28)</f>
         <v/>
       </c>
-      <c r="G29" s="109"/>
-      <c r="H29" s="110"/>
-      <c r="I29" s="111"/>
+      <c r="G29" s="109">
+        <v>0.25</v>
+      </c>
+      <c r="H29" s="110">
+        <v>1</v>
+      </c>
+      <c r="I29" s="111" t="s">
+        <v>97</v>
+      </c>
       <c r="M29" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -11785,17 +12161,17 @@
       <c r="R29" s="8"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B30" s="50" t="str">
+      <c r="B30" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B29)&lt;&gt;0,'Sprint 1 - Planification'!B29,"")</f>
-        <v/>
+        <v>22</v>
       </c>
       <c r="C30" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C29)&lt;&gt;0,'Sprint 1 - Planification'!C29,"")</f>
-        <v/>
+        <v>Créer l'animation des cartes</v>
       </c>
       <c r="D30" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H29)&lt;&gt;0,'Sprint 1 - Planification'!H29,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E30" s="67" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E29),"",'Sprint 1 - Bilan'!E29)</f>
@@ -11827,17 +12203,17 @@
       <c r="R30" s="8"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="53" t="str">
+      <c r="B31" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B30)&lt;&gt;0,'Sprint 1 - Planification'!B30,"")</f>
-        <v/>
+        <v>23</v>
       </c>
       <c r="C31" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C30)&lt;&gt;0,'Sprint 1 - Planification'!C30,"")</f>
-        <v/>
+        <v>Créer un UI pour le wild card</v>
       </c>
       <c r="D31" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H30)&lt;&gt;0,'Sprint 1 - Planification'!H30,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E31" s="69" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E30),"",'Sprint 1 - Bilan'!E30)</f>
@@ -11869,17 +12245,17 @@
       <c r="R31" s="8"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="50" t="str">
+      <c r="B32" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B31)&lt;&gt;0,'Sprint 1 - Planification'!B31,"")</f>
-        <v/>
+        <v>24</v>
       </c>
       <c r="C32" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C31)&lt;&gt;0,'Sprint 1 - Planification'!C31,"")</f>
-        <v/>
+        <v>créer un système de point</v>
       </c>
       <c r="D32" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H31)&lt;&gt;0,'Sprint 1 - Planification'!H31,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E32" s="67" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E31),"",'Sprint 1 - Bilan'!E31)</f>
@@ -12375,33 +12751,33 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>2 champs</v>
+        <v>1 champ</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -12576,8 +12952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:Z57"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12598,7 +12974,7 @@
     <row r="2" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="123" t="str">
         <f>'Sprint 1 - Planification'!B2:H2</f>
-        <v>Nom du projet super cool que vous faites!</v>
+        <v>UnoJS</v>
       </c>
       <c r="C2" s="123"/>
       <c r="D2" s="123"/>
@@ -12610,7 +12986,7 @@
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="33"/>
@@ -12632,7 +13008,7 @@
     </row>
     <row r="5" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
@@ -12642,32 +13018,32 @@
       <c r="H5" s="35"/>
       <c r="I5" s="64" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 2 champs à remplir!</v>
+        <v>Attention, il reste 6 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="131" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="129" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7" s="127" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="125" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F7" s="126"/>
       <c r="G7" s="131" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H7" s="133" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I7" s="135" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M7" s="7"/>
     </row>
@@ -12676,10 +13052,10 @@
       <c r="C8" s="130"/>
       <c r="D8" s="128"/>
       <c r="E8" s="119" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F8" s="119" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G8" s="132"/>
       <c r="H8" s="134"/>
@@ -12701,22 +13077,22 @@
       </c>
       <c r="E9" s="66">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E9)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G9)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E9)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G9))</f>
-        <v>1.0416666666666701E-2</v>
+        <v>2.0833333333333402E-2</v>
       </c>
       <c r="F9" s="65">
         <f>IF(LEN('Sprint 2 - Bilan'!$H9)&lt;&gt;0,'Sprint 2 - Bilan'!$H9,IF(LEN('Sprint 2 - Bilan'!$F9)=0,"",'Sprint 2 - Bilan'!$F9))</f>
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="G9" s="103"/>
       <c r="H9" s="104"/>
       <c r="I9" s="105"/>
       <c r="M9" s="3" t="b">
         <f>OR(AND(NOT(P9),LEN($G9)=0),AND(LEN($H9)&gt;0,LEN($G9)=0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="3" t="b">
         <f>AND(NOT($P9),LEN($H9)=0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" s="3" t="b">
         <f>AND(LEN($H9)&gt;0,$H9&lt;100%,LEN($I9)=0)</f>
@@ -12724,10 +13100,10 @@
       </c>
       <c r="P9" s="3" t="b">
         <f>IF(LEN($C9)=0,TRUE,IF(LEN($F9)=0,IF(LEN($H9)=0,FALSE,$H9=100%),IF($F9=100%,TRUE,IF(LEN($H9)=0,FALSE,$H9=100%))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="S9" s="61">
         <f t="array" ref="S9">SUM(($D$9:$D$43=$R9)*$G$9:$G$43)</f>
@@ -12739,7 +13115,7 @@
       </c>
       <c r="V9" s="9">
         <f>SUM(G9:G43)</f>
-        <v>0</v>
+        <v>1.4062500000000044</v>
       </c>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
@@ -12783,19 +13159,19 @@
         <v>1</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="S10" s="61">
         <f t="array" ref="S10">SUM(($D$9:$D$43=$R10)*$G$9:$G$43)</f>
-        <v>0</v>
+        <v>0.39583333333333304</v>
       </c>
       <c r="T10" s="62">
         <f t="shared" ref="T10:T11" si="4">S10*24*60</f>
-        <v>0</v>
+        <v>569.99999999999955</v>
       </c>
       <c r="V10" s="10">
         <f>V9</f>
-        <v>0</v>
+        <v>1.4062500000000044</v>
       </c>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
@@ -12839,19 +13215,19 @@
         <v>1</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S11" s="61">
         <f t="array" ref="S11">SUM(($D$9:$D$43=$R11)*$G$9:$G$43)</f>
-        <v>0</v>
+        <v>1.0104166666666716</v>
       </c>
       <c r="T11" s="62">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1455.0000000000073</v>
       </c>
       <c r="V11" s="63">
         <f>DAY(V9)*24+HOUR(V9)</f>
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -12898,29 +13274,29 @@
       <c r="R12" s="8"/>
       <c r="V12" s="4">
         <f>MINUTE(V9)</f>
-        <v>0</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="53" t="str">
+      <c r="B13" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B12)&lt;&gt;0,'Sprint 1 - Planification'!B12,"")</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="C13" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C12)&lt;&gt;0,'Sprint 1 - Planification'!C12,"")</f>
-        <v/>
+        <v>Creer une classe mère carte</v>
       </c>
       <c r="D13" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H12)&lt;&gt;0,'Sprint 1 - Planification'!H12,"")</f>
-        <v/>
-      </c>
-      <c r="E13" s="69" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E13" s="69">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E13)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G13)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E13)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G13))</f>
-        <v/>
-      </c>
-      <c r="F13" s="73" t="str">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="F13" s="73">
         <f>IF(LEN('Sprint 2 - Bilan'!$H13)&lt;&gt;0,'Sprint 2 - Bilan'!$H13,IF(LEN('Sprint 2 - Bilan'!$F13)=0,"",'Sprint 2 - Bilan'!$F13))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G13" s="112"/>
       <c r="H13" s="110"/>
@@ -12943,37 +13319,37 @@
       </c>
       <c r="R13" s="8"/>
       <c r="U13" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="V13" s="63">
         <f>V11</f>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="W13" s="4" t="str">
         <f>V13 &amp; " " &amp; U13 &amp; IF(V13 &gt; 1, "s", "")</f>
-        <v>0 heure</v>
+        <v>33 heures</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B14" s="50" t="str">
+      <c r="B14" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B13)&lt;&gt;0,'Sprint 1 - Planification'!B13,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="C14" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C13)&lt;&gt;0,'Sprint 1 - Planification'!C13,"")</f>
-        <v/>
+        <v>Creer une classe deck</v>
       </c>
       <c r="D14" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H13)&lt;&gt;0,'Sprint 1 - Planification'!H13,"")</f>
-        <v/>
-      </c>
-      <c r="E14" s="67" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E14" s="67">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E14)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G14)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E14)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G14))</f>
-        <v/>
-      </c>
-      <c r="F14" s="71" t="str">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="F14" s="71">
         <f>IF(LEN('Sprint 2 - Bilan'!$H14)&lt;&gt;0,'Sprint 2 - Bilan'!$H14,IF(LEN('Sprint 2 - Bilan'!$F14)=0,"",'Sprint 2 - Bilan'!$F14))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G14" s="106"/>
       <c r="H14" s="107"/>
@@ -12996,37 +13372,37 @@
       </c>
       <c r="R14" s="8"/>
       <c r="U14" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="V14" s="4">
         <f>V12</f>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="W14" s="4" t="str">
         <f>V14 &amp; " " &amp; U14 &amp; IF(V14 &gt; 1, "s", "")</f>
-        <v>0 minute</v>
+        <v>45 minutes</v>
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="53" t="str">
+      <c r="B15" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B14)&lt;&gt;0,'Sprint 1 - Planification'!B14,"")</f>
-        <v/>
+        <v>7</v>
       </c>
       <c r="C15" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C14)&lt;&gt;0,'Sprint 1 - Planification'!C14,"")</f>
-        <v/>
+        <v>creer une classe hand</v>
       </c>
       <c r="D15" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H14)&lt;&gt;0,'Sprint 1 - Planification'!H14,"")</f>
-        <v/>
-      </c>
-      <c r="E15" s="69" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E15" s="69">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E15)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G15)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E15)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G15))</f>
-        <v/>
-      </c>
-      <c r="F15" s="73" t="str">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F15" s="73">
         <f>IF(LEN('Sprint 2 - Bilan'!$H15)&lt;&gt;0,'Sprint 2 - Bilan'!$H15,IF(LEN('Sprint 2 - Bilan'!$F15)=0,"",'Sprint 2 - Bilan'!$F15))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G15" s="112"/>
       <c r="H15" s="110"/>
@@ -13050,36 +13426,40 @@
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
         <f>IF(V13&gt;0,IF(V14&gt;0,W13&amp;" et "&amp;W14,W13),W14)</f>
-        <v>0 minute</v>
+        <v>33 heures et 45 minutes</v>
       </c>
       <c r="Y15" s="4" t="str">
         <f>V13&amp;"h"&amp;TEXT(V14,"00")</f>
-        <v>0h00</v>
+        <v>33h45</v>
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B16" s="50" t="str">
+      <c r="B16" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B15)&lt;&gt;0,'Sprint 1 - Planification'!B15,"")</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="C16" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C15)&lt;&gt;0,'Sprint 1 - Planification'!C15,"")</f>
-        <v/>
+        <v>creer une classe joueur</v>
       </c>
       <c r="D16" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H15)&lt;&gt;0,'Sprint 1 - Planification'!H15,"")</f>
-        <v/>
-      </c>
-      <c r="E16" s="67" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E16" s="67">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E16)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G16)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E16)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G16))</f>
-        <v/>
-      </c>
-      <c r="F16" s="71" t="str">
+        <v>0.125</v>
+      </c>
+      <c r="F16" s="71">
         <f>IF(LEN('Sprint 2 - Bilan'!$H16)&lt;&gt;0,'Sprint 2 - Bilan'!$H16,IF(LEN('Sprint 2 - Bilan'!$F16)=0,"",'Sprint 2 - Bilan'!$F16))</f>
-        <v/>
-      </c>
-      <c r="G16" s="106"/>
-      <c r="H16" s="107"/>
+        <v>0.9</v>
+      </c>
+      <c r="G16" s="106">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H16" s="107">
+        <v>1</v>
+      </c>
       <c r="I16" s="108"/>
       <c r="M16" s="3" t="b">
         <f t="shared" si="0"/>
@@ -13100,36 +13480,40 @@
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche n'a pas été terminée!",CONCATENATE(V16," tâches n'ont pas été terminé!")))</f>
-        <v>Une tâche n'a pas été terminée!</v>
+        <v>4 tâches n'ont pas été terminé!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="53" t="str">
+      <c r="B17" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B16)&lt;&gt;0,'Sprint 1 - Planification'!B16,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="C17" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C16)&lt;&gt;0,'Sprint 1 - Planification'!C16,"")</f>
-        <v/>
+        <v>creer une classe table</v>
       </c>
       <c r="D17" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H16)&lt;&gt;0,'Sprint 1 - Planification'!H16,"")</f>
-        <v/>
-      </c>
-      <c r="E17" s="68" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E17" s="68">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E17)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G17)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E17)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G17))</f>
-        <v/>
-      </c>
-      <c r="F17" s="72" t="str">
+        <v>0.14583333333333301</v>
+      </c>
+      <c r="F17" s="72">
         <f>IF(LEN('Sprint 2 - Bilan'!$H17)&lt;&gt;0,'Sprint 2 - Bilan'!$H17,IF(LEN('Sprint 2 - Bilan'!$F17)=0,"",'Sprint 2 - Bilan'!$F17))</f>
-        <v/>
-      </c>
-      <c r="G17" s="109"/>
-      <c r="H17" s="110"/>
+        <v>0.8</v>
+      </c>
+      <c r="G17" s="109">
+        <v>0.125</v>
+      </c>
+      <c r="H17" s="110">
+        <v>1</v>
+      </c>
       <c r="I17" s="111"/>
       <c r="M17" s="3" t="b">
         <f t="shared" si="0"/>
@@ -13150,25 +13534,25 @@
       <c r="R17" s="8"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="50" t="str">
+      <c r="B18" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B17)&lt;&gt;0,'Sprint 1 - Planification'!B17,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="C18" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C17)&lt;&gt;0,'Sprint 1 - Planification'!C17,"")</f>
-        <v/>
+        <v>creer une variable globale jeu</v>
       </c>
       <c r="D18" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H17)&lt;&gt;0,'Sprint 1 - Planification'!H17,"")</f>
-        <v/>
-      </c>
-      <c r="E18" s="67" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E18" s="67">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E18)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G18)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E18)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G18))</f>
-        <v/>
-      </c>
-      <c r="F18" s="71" t="str">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="F18" s="71">
         <f>IF(LEN('Sprint 2 - Bilan'!$H18)&lt;&gt;0,'Sprint 2 - Bilan'!$H18,IF(LEN('Sprint 2 - Bilan'!$F18)=0,"",'Sprint 2 - Bilan'!$F18))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G18" s="106"/>
       <c r="H18" s="107"/>
@@ -13192,29 +13576,35 @@
       <c r="R18" s="8"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="53" t="str">
+      <c r="B19" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B18)&lt;&gt;0,'Sprint 1 - Planification'!B18,"")</f>
-        <v/>
+        <v>11</v>
       </c>
       <c r="C19" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C18)&lt;&gt;0,'Sprint 1 - Planification'!C18,"")</f>
-        <v/>
+        <v>creer une classe règles</v>
       </c>
       <c r="D19" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H18)&lt;&gt;0,'Sprint 1 - Planification'!H18,"")</f>
-        <v/>
-      </c>
-      <c r="E19" s="69" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E19" s="69">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E19)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G19)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E19)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G19))</f>
-        <v/>
-      </c>
-      <c r="F19" s="73" t="str">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="F19" s="73">
         <f>IF(LEN('Sprint 2 - Bilan'!$H19)&lt;&gt;0,'Sprint 2 - Bilan'!$H19,IF(LEN('Sprint 2 - Bilan'!$F19)=0,"",'Sprint 2 - Bilan'!$F19))</f>
-        <v/>
-      </c>
-      <c r="G19" s="112"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="111"/>
+        <v>0.7</v>
+      </c>
+      <c r="G19" s="112">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="H19" s="110">
+        <v>1</v>
+      </c>
+      <c r="I19" s="111" t="s">
+        <v>104</v>
+      </c>
       <c r="M19" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -13234,17 +13624,17 @@
       <c r="R19" s="8"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="50" t="str">
+      <c r="B20" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B19)&lt;&gt;0,'Sprint 1 - Planification'!B19,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="C20" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C19)&lt;&gt;0,'Sprint 1 - Planification'!C19,"")</f>
-        <v/>
+        <v>creer un lobby</v>
       </c>
       <c r="D20" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H19)&lt;&gt;0,'Sprint 1 - Planification'!H19,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E20" s="67" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E20)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G20)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E20)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G20))</f>
@@ -13254,9 +13644,15 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H20)&lt;&gt;0,'Sprint 2 - Bilan'!$H20,IF(LEN('Sprint 2 - Bilan'!$F20)=0,"",'Sprint 2 - Bilan'!$F20))</f>
         <v/>
       </c>
-      <c r="G20" s="106"/>
-      <c r="H20" s="107"/>
-      <c r="I20" s="108"/>
+      <c r="G20" s="106">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="H20" s="107">
+        <v>1</v>
+      </c>
+      <c r="I20" s="108" t="s">
+        <v>99</v>
+      </c>
       <c r="M20" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -13276,17 +13672,17 @@
       <c r="R20" s="8"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="53" t="str">
+      <c r="B21" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B20)&lt;&gt;0,'Sprint 1 - Planification'!B20,"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C21" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C20)&lt;&gt;0,'Sprint 1 - Planification'!C20,"")</f>
-        <v/>
+        <v>créer un menu</v>
       </c>
       <c r="D21" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H20)&lt;&gt;0,'Sprint 1 - Planification'!H20,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E21" s="69" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E21)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G21)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E21)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G21))</f>
@@ -13296,9 +13692,15 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H21)&lt;&gt;0,'Sprint 2 - Bilan'!$H21,IF(LEN('Sprint 2 - Bilan'!$F21)=0,"",'Sprint 2 - Bilan'!$F21))</f>
         <v/>
       </c>
-      <c r="G21" s="112"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="111"/>
+      <c r="G21" s="112">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H21" s="110">
+        <v>1</v>
+      </c>
+      <c r="I21" s="111" t="s">
+        <v>102</v>
+      </c>
       <c r="M21" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -13318,17 +13720,17 @@
       <c r="R21" s="8"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="50" t="str">
+      <c r="B22" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B21)&lt;&gt;0,'Sprint 1 - Planification'!B21,"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C22" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C21)&lt;&gt;0,'Sprint 1 - Planification'!C21,"")</f>
-        <v/>
+        <v>créer mécanique UNO</v>
       </c>
       <c r="D22" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H21)&lt;&gt;0,'Sprint 1 - Planification'!H21,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E22" s="67" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E22)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G22)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E22)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G22))</f>
@@ -13339,11 +13741,13 @@
         <v/>
       </c>
       <c r="G22" s="106"/>
-      <c r="H22" s="107"/>
+      <c r="H22" s="107">
+        <v>0</v>
+      </c>
       <c r="I22" s="108"/>
       <c r="M22" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="3" t="b">
         <f t="shared" si="1"/>
@@ -13351,34 +13755,34 @@
       </c>
       <c r="O22" s="3" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P22" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22" s="8"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="53" t="str">
+      <c r="B23" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B22)&lt;&gt;0,'Sprint 1 - Planification'!B22,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C23" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C22)&lt;&gt;0,'Sprint 1 - Planification'!C22,"")</f>
-        <v/>
+        <v>implémenter un random des cartes</v>
       </c>
       <c r="D23" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H22)&lt;&gt;0,'Sprint 1 - Planification'!H22,"")</f>
-        <v/>
-      </c>
-      <c r="E23" s="68" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E23" s="68">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E23)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G23)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E23)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G23))</f>
-        <v/>
-      </c>
-      <c r="F23" s="72" t="str">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="F23" s="72">
         <f>IF(LEN('Sprint 2 - Bilan'!$H23)&lt;&gt;0,'Sprint 2 - Bilan'!$H23,IF(LEN('Sprint 2 - Bilan'!$F23)=0,"",'Sprint 2 - Bilan'!$F23))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G23" s="109"/>
       <c r="H23" s="110"/>
@@ -13402,17 +13806,17 @@
       <c r="R23" s="8"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="50" t="str">
+      <c r="B24" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B23)&lt;&gt;0,'Sprint 1 - Planification'!B23,"")</f>
-        <v/>
+        <v>16</v>
       </c>
       <c r="C24" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C23)&lt;&gt;0,'Sprint 1 - Planification'!C23,"")</f>
-        <v/>
+        <v>créer un algorithme d'affichage des joueurs</v>
       </c>
       <c r="D24" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H23)&lt;&gt;0,'Sprint 1 - Planification'!H23,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E24" s="67" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E24)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G24)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E24)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G24))</f>
@@ -13422,8 +13826,12 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H24)&lt;&gt;0,'Sprint 2 - Bilan'!$H24,IF(LEN('Sprint 2 - Bilan'!$F24)=0,"",'Sprint 2 - Bilan'!$F24))</f>
         <v/>
       </c>
-      <c r="G24" s="106"/>
-      <c r="H24" s="107"/>
+      <c r="G24" s="106">
+        <v>0.13541666666666699</v>
+      </c>
+      <c r="H24" s="107">
+        <v>1</v>
+      </c>
       <c r="I24" s="108"/>
       <c r="M24" s="3" t="b">
         <f t="shared" si="0"/>
@@ -13444,17 +13852,17 @@
       <c r="R24" s="8"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="53" t="str">
+      <c r="B25" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B24)&lt;&gt;0,'Sprint 1 - Planification'!B24,"")</f>
-        <v/>
+        <v>17</v>
       </c>
       <c r="C25" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C24)&lt;&gt;0,'Sprint 1 - Planification'!C24,"")</f>
-        <v/>
+        <v>Créer le code reliant client-serveur</v>
       </c>
       <c r="D25" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H24)&lt;&gt;0,'Sprint 1 - Planification'!H24,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E25" s="69" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E25)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G25)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E25)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G25))</f>
@@ -13464,9 +13872,15 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H25)&lt;&gt;0,'Sprint 2 - Bilan'!$H25,IF(LEN('Sprint 2 - Bilan'!$F25)=0,"",'Sprint 2 - Bilan'!$F25))</f>
         <v/>
       </c>
-      <c r="G25" s="112"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="111"/>
+      <c r="G25" s="112">
+        <v>0.51041666666667096</v>
+      </c>
+      <c r="H25" s="110">
+        <v>1</v>
+      </c>
+      <c r="I25" s="111" t="s">
+        <v>100</v>
+      </c>
       <c r="M25" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -13486,17 +13900,17 @@
       <c r="R25" s="8"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="50" t="str">
+      <c r="B26" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B25)&lt;&gt;0,'Sprint 1 - Planification'!B25,"")</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="C26" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C25)&lt;&gt;0,'Sprint 1 - Planification'!C25,"")</f>
-        <v/>
+        <v>Se procurer un serveur</v>
       </c>
       <c r="D26" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H25)&lt;&gt;0,'Sprint 1 - Planification'!H25,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E26" s="67" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E26)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G26)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E26)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G26))</f>
@@ -13507,11 +13921,13 @@
         <v/>
       </c>
       <c r="G26" s="106"/>
-      <c r="H26" s="107"/>
+      <c r="H26" s="107">
+        <v>0</v>
+      </c>
       <c r="I26" s="108"/>
       <c r="M26" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="3" t="b">
         <f t="shared" si="1"/>
@@ -13519,26 +13935,26 @@
       </c>
       <c r="O26" s="3" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R26" s="8"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="53" t="str">
+      <c r="B27" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B26)&lt;&gt;0,'Sprint 1 - Planification'!B26,"")</f>
-        <v/>
+        <v>19</v>
       </c>
       <c r="C27" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v/>
+        <v>Créer un menu d'options</v>
       </c>
       <c r="D27" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E27" s="69" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E27)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G27)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E27)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G27))</f>
@@ -13549,11 +13965,15 @@
         <v/>
       </c>
       <c r="G27" s="112"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="111"/>
+      <c r="H27" s="110">
+        <v>0</v>
+      </c>
+      <c r="I27" s="111" t="s">
+        <v>105</v>
+      </c>
       <c r="M27" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27" s="3" t="b">
         <f t="shared" si="1"/>
@@ -13565,30 +13985,30 @@
       </c>
       <c r="P27" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27" s="8"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="50" t="str">
+      <c r="B28" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B27)&lt;&gt;0,'Sprint 1 - Planification'!B27,"")</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="C28" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C27)&lt;&gt;0,'Sprint 1 - Planification'!C27,"")</f>
-        <v/>
+        <v>Créer un UI de gameplay</v>
       </c>
       <c r="D28" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H27)&lt;&gt;0,'Sprint 1 - Planification'!H27,"")</f>
-        <v/>
-      </c>
-      <c r="E28" s="67" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E28" s="67">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E28)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G28)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E28)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G28))</f>
-        <v/>
-      </c>
-      <c r="F28" s="71" t="str">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="F28" s="71">
         <f>IF(LEN('Sprint 2 - Bilan'!$H28)&lt;&gt;0,'Sprint 2 - Bilan'!$H28,IF(LEN('Sprint 2 - Bilan'!$F28)=0,"",'Sprint 2 - Bilan'!$F28))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G28" s="106"/>
       <c r="H28" s="107"/>
@@ -13612,25 +14032,25 @@
       <c r="R28" s="8"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="53" t="str">
+      <c r="B29" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B28)&lt;&gt;0,'Sprint 1 - Planification'!B28,"")</f>
-        <v/>
+        <v>21</v>
       </c>
       <c r="C29" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C28)&lt;&gt;0,'Sprint 1 - Planification'!C28,"")</f>
-        <v/>
+        <v>Créer un UI pour la carte</v>
       </c>
       <c r="D29" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H28)&lt;&gt;0,'Sprint 1 - Planification'!H28,"")</f>
-        <v/>
-      </c>
-      <c r="E29" s="68" t="str">
+        <v>Sprint 2</v>
+      </c>
+      <c r="E29" s="68">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E29)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G29)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E29)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G29))</f>
-        <v/>
-      </c>
-      <c r="F29" s="72" t="str">
+        <v>0.25</v>
+      </c>
+      <c r="F29" s="72">
         <f>IF(LEN('Sprint 2 - Bilan'!$H29)&lt;&gt;0,'Sprint 2 - Bilan'!$H29,IF(LEN('Sprint 2 - Bilan'!$F29)=0,"",'Sprint 2 - Bilan'!$F29))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G29" s="109"/>
       <c r="H29" s="110"/>
@@ -13654,17 +14074,17 @@
       <c r="R29" s="8"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B30" s="50" t="str">
+      <c r="B30" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B29)&lt;&gt;0,'Sprint 1 - Planification'!B29,"")</f>
-        <v/>
+        <v>22</v>
       </c>
       <c r="C30" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C29)&lt;&gt;0,'Sprint 1 - Planification'!C29,"")</f>
-        <v/>
+        <v>Créer l'animation des cartes</v>
       </c>
       <c r="D30" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H29)&lt;&gt;0,'Sprint 1 - Planification'!H29,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E30" s="67" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E30)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G30)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E30)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G30))</f>
@@ -13674,8 +14094,12 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H30)&lt;&gt;0,'Sprint 2 - Bilan'!$H30,IF(LEN('Sprint 2 - Bilan'!$F30)=0,"",'Sprint 2 - Bilan'!$F30))</f>
         <v/>
       </c>
-      <c r="G30" s="106"/>
-      <c r="H30" s="107"/>
+      <c r="G30" s="106">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H30" s="107">
+        <v>1</v>
+      </c>
       <c r="I30" s="108"/>
       <c r="M30" s="3" t="b">
         <f t="shared" si="0"/>
@@ -13696,17 +14120,17 @@
       <c r="R30" s="8"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="53" t="str">
+      <c r="B31" s="53">
         <f>IF(LEN('Sprint 1 - Planification'!B30)&lt;&gt;0,'Sprint 1 - Planification'!B30,"")</f>
-        <v/>
+        <v>23</v>
       </c>
       <c r="C31" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C30)&lt;&gt;0,'Sprint 1 - Planification'!C30,"")</f>
-        <v/>
+        <v>Créer un UI pour le wild card</v>
       </c>
       <c r="D31" s="56" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H30)&lt;&gt;0,'Sprint 1 - Planification'!H30,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E31" s="69" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E31)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G31)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E31)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G31))</f>
@@ -13716,9 +14140,15 @@
         <f>IF(LEN('Sprint 2 - Bilan'!$H31)&lt;&gt;0,'Sprint 2 - Bilan'!$H31,IF(LEN('Sprint 2 - Bilan'!$F31)=0,"",'Sprint 2 - Bilan'!$F31))</f>
         <v/>
       </c>
-      <c r="G31" s="112"/>
-      <c r="H31" s="110"/>
-      <c r="I31" s="111"/>
+      <c r="G31" s="112">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H31" s="110">
+        <v>1</v>
+      </c>
+      <c r="I31" s="111" t="s">
+        <v>103</v>
+      </c>
       <c r="M31" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -13738,17 +14168,17 @@
       <c r="R31" s="8"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="50" t="str">
+      <c r="B32" s="50">
         <f>IF(LEN('Sprint 1 - Planification'!B31)&lt;&gt;0,'Sprint 1 - Planification'!B31,"")</f>
-        <v/>
+        <v>24</v>
       </c>
       <c r="C32" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C31)&lt;&gt;0,'Sprint 1 - Planification'!C31,"")</f>
-        <v/>
+        <v>créer un système de point</v>
       </c>
       <c r="D32" s="52" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H31)&lt;&gt;0,'Sprint 1 - Planification'!H31,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E32" s="67" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E32)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G32)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E32)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G32))</f>
@@ -13759,11 +14189,15 @@
         <v/>
       </c>
       <c r="G32" s="106"/>
-      <c r="H32" s="107"/>
-      <c r="I32" s="108"/>
+      <c r="H32" s="107">
+        <v>0</v>
+      </c>
+      <c r="I32" s="108" t="s">
+        <v>106</v>
+      </c>
       <c r="M32" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N32" s="3" t="b">
         <f t="shared" si="1"/>
@@ -13775,7 +14209,7 @@
       </c>
       <c r="P32" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R32" s="8"/>
     </row>
@@ -14244,33 +14678,33 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>2 champs</v>
+        <v>6 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -14413,7 +14847,7 @@
     <row r="1" spans="2:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="102" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="102"/>
       <c r="D2" s="102"/>
@@ -14426,7 +14860,7 @@
     </row>
     <row r="3" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="82"/>
       <c r="D3" s="82"/>
@@ -14442,7 +14876,7 @@
     </row>
     <row r="5" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="81" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="83"/>
       <c r="D5" s="83"/>
@@ -14457,16 +14891,16 @@
     <row r="7" spans="2:25" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B7" s="87"/>
       <c r="C7" s="88" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="88" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="88" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="88" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -14481,7 +14915,7 @@
     </row>
     <row r="8" spans="2:25" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B8" s="85" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C8" s="89">
         <f>L8</f>
@@ -14489,15 +14923,15 @@
       </c>
       <c r="D8" s="90">
         <f>M8</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E8" s="91">
         <f>N8</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F8" s="95">
         <f>O8</f>
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -14507,15 +14941,15 @@
       </c>
       <c r="M8" s="1">
         <f>'Sprint 1 - Planification'!AJ18</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1">
         <f>'Sprint 1 - Planification'!AJ19</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O8" s="1">
         <f>SUM(L8:N8)</f>
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -14524,7 +14958,7 @@
     </row>
     <row r="9" spans="2:25" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B9" s="86" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="92" t="str">
         <f t="shared" ref="C9:F10" si="0">DAY(L9)*24+HOUR(L9)&amp;"h"&amp;TEXT(MINUTE(L9),"00")</f>
@@ -14532,15 +14966,15 @@
       </c>
       <c r="D9" s="93" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>15h45</v>
       </c>
       <c r="E9" s="94" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>24h00</v>
       </c>
       <c r="F9" s="96" t="str">
         <f t="shared" si="0"/>
-        <v>12h30</v>
+        <v>52h15</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -14550,18 +14984,18 @@
       </c>
       <c r="M9" s="1">
         <f>'Sprint 1 - Planification'!AD18</f>
-        <v>0</v>
+        <v>0.65625000000000011</v>
       </c>
       <c r="N9" s="1">
         <f>'Sprint 1 - Planification'!AD19</f>
-        <v>0</v>
+        <v>1.0000000000000004</v>
       </c>
       <c r="O9" s="1">
         <f>SUM(L9:N9)</f>
-        <v>0.5208333333333337</v>
+        <v>2.1770833333333344</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="Q9" s="1">
         <f t="shared" ref="Q9:S10" si="1">DAY(L9)*24+HOUR(L9)+MINUTE(L9)/60</f>
@@ -14569,30 +15003,30 @@
       </c>
       <c r="R9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15.75</v>
       </c>
       <c r="S9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="V9" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!E8:E42,"Essentielle")</f>
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Y9" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!F8:F42,1)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:25" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B10" s="85" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="89" t="str">
         <f t="shared" si="0"/>
@@ -14600,15 +15034,15 @@
       </c>
       <c r="D10" s="90" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>26h00</v>
       </c>
       <c r="E10" s="91" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>33h45</v>
       </c>
       <c r="F10" s="95" t="str">
         <f t="shared" si="0"/>
-        <v>2h15</v>
+        <v>62h00</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -14618,18 +15052,18 @@
       </c>
       <c r="M10" s="1">
         <f>'Sprint 2 - Bilan'!V9</f>
-        <v>0</v>
+        <v>1.0833333333333326</v>
       </c>
       <c r="N10" s="1">
         <f>'Sprint 3 - Bilan'!V9</f>
-        <v>0</v>
+        <v>1.4062500000000044</v>
       </c>
       <c r="O10" s="1">
         <f>SUM(L10:N10)</f>
-        <v>9.3749999999999972E-2</v>
+        <v>2.583333333333337</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="1"/>
@@ -14637,30 +15071,30 @@
       </c>
       <c r="R10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="S10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>33.75</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="V10" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!E8:E42,"Optionnelle")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Y10" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!F8:F42,2)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:25" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="97" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="98">
         <f>L11</f>
@@ -14668,15 +15102,15 @@
       </c>
       <c r="D11" s="99">
         <f>M11</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11" s="100">
         <f>N11</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F11" s="101">
         <f>O11</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -14686,26 +15120,26 @@
       </c>
       <c r="M11" s="1">
         <f>'Sprint 2 - Bilan'!V16</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N11" s="1">
         <f>'Sprint 3 - Bilan'!V16</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O11" s="1">
         <f>N11</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="X11" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Y11" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!F8:F42,3)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:25" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -14859,7 +15293,7 @@
     <row r="1" spans="2:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="137" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="137"/>
       <c r="D2" s="137"/>
@@ -14870,7 +15304,7 @@
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="75"/>
@@ -14890,7 +15324,7 @@
     </row>
     <row r="5" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="77"/>
@@ -14903,7 +15337,7 @@
     <row r="7" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="79" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="78"/>
       <c r="E7" s="1"/>
@@ -14914,7 +15348,7 @@
     <row r="8" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B8" s="78"/>
       <c r="D8" s="78" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -14924,7 +15358,7 @@
     <row r="9" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="D9" s="78" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -14942,7 +15376,7 @@
     <row r="11" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="79" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="78"/>
       <c r="E11" s="1"/>
@@ -14953,7 +15387,7 @@
     <row r="12" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="D12" s="78" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -14963,7 +15397,7 @@
     <row r="13" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="D13" s="78" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -14973,7 +15407,7 @@
     <row r="14" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="D14" s="78" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -14983,7 +15417,7 @@
     <row r="15" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="D15" s="78" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -14993,7 +15427,7 @@
     <row r="16" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="D16" s="78" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -15003,7 +15437,7 @@
     <row r="17" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="D17" s="78" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -15013,7 +15447,7 @@
     <row r="18" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="D18" s="78" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -15022,7 +15456,7 @@
     </row>
     <row r="20" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="77"/>
@@ -15035,7 +15469,7 @@
     <row r="22" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="79" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D22" s="78"/>
       <c r="E22" s="1"/>
@@ -15046,7 +15480,7 @@
     <row r="23" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B23" s="78"/>
       <c r="D23" s="78" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -15056,7 +15490,7 @@
     <row r="24" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="D24" s="78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -15066,7 +15500,7 @@
     <row r="25" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="D25" s="78" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -15083,7 +15517,7 @@
     </row>
     <row r="28" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="77"/>
@@ -15096,7 +15530,7 @@
     <row r="30" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="79" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D30" s="78"/>
       <c r="E30" s="1"/>
@@ -15114,7 +15548,7 @@
     </row>
     <row r="33" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="77"/>
@@ -15127,7 +15561,7 @@
     <row r="35" spans="2:8" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="138" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D35" s="138"/>
       <c r="E35" s="138"/>
@@ -15176,21 +15610,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F62C6454CE4AC42BDCAC344ECDB29E7" ma:contentTypeVersion="5" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="041f2529e877cf445b142ab8b85103c0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="78692225-e198-47c3-adde-2ea492f0b3f0" xmlns:ns3="9fb5ff05-ea2d-4c6e-ac8e-f51bc8309790" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d896ed1249059892348595dbe15b813f" ns2:_="" ns3:_="">
     <xsd:import namespace="78692225-e198-47c3-adde-2ea492f0b3f0"/>
@@ -15361,24 +15780,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20DD170F-C51C-4776-BE86-DE3613560936}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16325D0D-63D9-490D-8587-E384C7BFA0C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6429BCA9-91E9-4F0E-9921-9689A9C725AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15395,4 +15812,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16325D0D-63D9-490D-8587-E384C7BFA0C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20DD170F-C51C-4776-BE86-DE3613560936}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>